<commit_message>
PCB ready for final review
</commit_message>
<xml_diff>
--- a/References/Buck parts calculation.xlsx
+++ b/References/Buck parts calculation.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvicca0-my.sharepoint.com/personal/poornack_uvic_ca/Documents/University/Clubs/AUVic/PCB/Weight_Dropper_Torpedo_1.0_PCB/References/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Poorna\OneDrive - University of Victoria\University\Clubs\AUVic\PCB\Weight_Dropper_Torpedo_1.0_PCB\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="10046"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="10046" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LM2576" sheetId="1" r:id="rId1"/>
+    <sheet name="LM2596" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Inductor</t>
   </si>
@@ -99,6 +100,42 @@
   </si>
   <si>
     <t>470uF</t>
+  </si>
+  <si>
+    <t>TOO BIG</t>
+  </si>
+  <si>
+    <t>150uH</t>
+  </si>
+  <si>
+    <t>3.5A</t>
+  </si>
+  <si>
+    <t>47uH</t>
+  </si>
+  <si>
+    <t>732-1246-1-ND</t>
+  </si>
+  <si>
+    <t>18V</t>
+  </si>
+  <si>
+    <t>150uF</t>
+  </si>
+  <si>
+    <t>PCE5017CT-ND</t>
+  </si>
+  <si>
+    <t>40V</t>
+  </si>
+  <si>
+    <t>470uH</t>
+  </si>
+  <si>
+    <t>P12400-ND</t>
+  </si>
+  <si>
+    <t>LM2596</t>
   </si>
 </sst>
 </file>
@@ -481,10 +518,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F19"/>
+  <dimension ref="A2:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.61328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <f>1.15*B4</f>
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <f>1.5*B3</f>
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f>1.2*B4</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="C15">
+        <f>1.2*B2</f>
+        <v>30.24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <f>B2</f>
+        <v>25.2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3">
+        <f>SUM(F8:F18)</f>
+        <v>5.74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="E12" r:id="rId2"/>
+    <hyperlink ref="E15" r:id="rId3"/>
+    <hyperlink ref="E18" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -503,6 +736,9 @@
       <c r="B2">
         <v>25.2</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
@@ -538,131 +774,128 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8">
-        <f>1.15*B4</f>
-        <v>3.4499999999999997</v>
+      <c r="B8" t="s">
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4">
-        <v>3.69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <f>1.5*B3</f>
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+    <row r="15" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <f>1.2*B4</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f>1.2*B2</f>
         <v>30.24</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F15" s="4">
         <v>0.59</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+    <row r="18" spans="1:6" ht="15.45" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <f>B2</f>
-        <v>25.2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="E19" t="s">
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="3">
-        <f>SUM(F8:F17)</f>
-        <v>5.74</v>
+      <c r="F20" s="3">
+        <f>SUM(F8:F18)</f>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E11" r:id="rId2"/>
-    <hyperlink ref="E14" r:id="rId3"/>
-    <hyperlink ref="E17" r:id="rId4"/>
+    <hyperlink ref="E12" r:id="rId1"/>
+    <hyperlink ref="E15" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>